<commit_message>
Add missing dissertations and Wetterhahn posters (Issue #6)
Added to publications:
- Owen LLW (2021) dissertation: "Modeling the fast-timescale network dynamics that underlie complex thought"
- Ziman K (2022) dissertation: "Attending and remembering the external world"
- Carstensen et al. (2024) Wetterhahn poster: EEG-based knowledge estimation
- Jha et al. (2023) Wetterhahn poster: High-order network dynamics

Total publications: 108 (was 104)
- Dissertations: 4 (was 2)
- Posters: 44 (was 42)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/publications.xlsx
+++ b/data/publications.xlsx
@@ -1604,7 +1604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1699,6 +1699,36 @@
           <t>[&lt;a href="http://caligari.dartmouth.edu/~jmanning/pubs/magellan_dissertation.pdf" target="_blank"&gt;PDF&lt;/a&gt;]</t>
         </is>
       </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Modeling the fast-timescale network dynamics that underlie complex thought</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Owen LLW (2021) Modeling the fast-timescale network dynamics that underlie complex thought. &lt;em&gt;Doctoral dissertation: Dartmouth College&lt;/em&gt;, Hanover, NH.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Attending and remembering the external world</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Ziman K (2022) Attending and remembering the external world. &lt;em&gt;Doctoral dissertation: Dartmouth College&lt;/em&gt;, Hanover, NH.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1774,7 +1804,6 @@
           <t>Manning (2021) Towards an exercise recommendation system for optimizing mental fitness. Talk given at the &lt;a href="https://www.c4tbh.org" target="_blank"&gt;&lt;em&gt;Center for Technology and Behavioral Health&lt;/em&gt;&lt;/a&gt;.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1797,7 +1826,6 @@
           <t>Manning (2020) Dynamic geometries of thoughts, memories, and conversations. Talk given at the &lt;a href="https://psychology.berkeley.edu/events/human-cognition-colloquium-2" target="_blank"&gt;&lt;em&gt;Human Cognition Colloquium&lt;/em&gt; at Berkeley&lt;/a&gt;.</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1820,7 +1848,6 @@
           <t>Manning (2019) Can we improve real-world learning using scalable AI teachers? Talk given at the &lt;a href="https://summer-mind.github.io/" target="_blank"&gt;&lt;em&gt;MIND Summer School at Dartmouth&lt;/em&gt;&lt;/a&gt;.</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1843,7 +1870,6 @@
           <t>Manning (2019) Coding like a rock star. Talk given at the &lt;a href="https://summer-mind.github.io/" target="_blank"&gt;&lt;em&gt;MIND Summer School at Dartmouth&lt;/em&gt;&lt;/a&gt;.</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1893,7 +1919,6 @@
           <t>Manning (2018) Contextual Dynamics. Talk given at the &lt;a href="https://summer-mind.github.io/" target="_blank"&gt;&lt;em&gt;MIND Summer School at Dartmouth&lt;/em&gt;&lt;/a&gt;.</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1943,7 +1968,6 @@
           <t>Manning (2018) Coding like a science hacker. Talk given at the &lt;a href="https://summer-mind.github.io/" target="_blank"&gt;&lt;em&gt;MIND Summer School at Dartmouth&lt;/em&gt;&lt;/a&gt;.</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2020,7 +2044,6 @@
           <t>Manning JR (2017) Towards human SuperEEG. Virtual talk given to the &lt;em&gt;&lt;a href="https://www.attentioninthebrain.com/" target="_blank"&gt;EPSCoR Attention Consortium&lt;/a&gt;&lt;/em&gt;.</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2043,7 +2066,6 @@
           <t>Manning JR (2015) A neural signature of mental time travel. Talk given at &lt;em&gt;Dartmouth-Hitchcock Medical Center Grand Rounds&lt;/em&gt;, Hanover, NH.</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2325,7 +2347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2388,7 +2410,6 @@
           <t>Ziman K, Lee MR, Martinez AR, Manning JR (2019) Volitional Attention Modulates Memory Encoding and Retrieval. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Chicago, IL</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2411,7 +2432,6 @@
           <t>Fitzpatrick PC, Heusser AC, Manning JR (2019) Exploring the evolving geometric structure of experiences and memories. &lt;em&gt;Society for Neuroscience&lt;/em&gt;. Chicago, IL.</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2434,7 +2454,6 @@
           <t>Owen LLW, Manning JR (2019) Understanding complexity and interactivity of brain patterns in naturalistic processing. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Chicago, IL.</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2457,7 +2476,6 @@
           <t>Heusser AC, Manning JR (2018) Capturing the geometric structure of episodic memories for naturalistic experiences. &lt;em&gt;Conference on Cognitive Computational Neuroscience&lt;/em&gt;, PS-2B.16.</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2480,7 +2498,6 @@
           <t>Ziman K, Lee MR, Martinez AR, Manning JR (2018) Volitional Attention Modulates Memory Encoding and Retrieval. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; San Diego, CA.</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2503,7 +2520,6 @@
           <t>Fitzpatrick PC, Heusser AC, Manning JR (2018) Mapping between naturalistic experience and verbal recall. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; San Diego, CA.</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2526,7 +2542,6 @@
           <t>Fitzpatrick PC, Ziman K, Heusser AC, Field CE, Manning JR (2018) The utility of speech-to-text software for transcription of verbal response data. &lt;em&gt;Wetterhan Science Symposium&lt;/em&gt;. Hanover, NH.</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2549,7 +2564,6 @@
           <t>Pak EK, Ziman K, Manning JR (2018) How does attention affect memory? &lt;em&gt;Wetterhan Science Symposium&lt;/em&gt;. Hanover, NH.</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2572,7 +2586,6 @@
           <t>Lee MR, Chacko RS, Whitaker EC, Fitzpatrick PC, Field CE, Ziman K, Bollinger BJ, Heusser AC, Manning JR (2018) Adaptive Free Recall: Enhancing (Or Diminishing) Memory. &lt;em&gt;Wetterhan Science Symposium&lt;/em&gt;. Hanover, NH.</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2595,7 +2608,6 @@
           <t>Heusser AC, Manning JR (2018) Modeling the dynamic content, encoding, and retrieval of naturalistic stimuli. &lt;em&gt;Cognitive Neuroscience Society.&lt;/em&gt; Boston, MA.</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2618,7 +2630,6 @@
           <t>Manning JR, Ziman K, Heusser AC (2017) Efficient Learning: Manipulating context to enhance (or diminish) memory. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2641,7 +2652,6 @@
           <t>Heusser AC, Ziman K, Owen LLW, Manning JR (2017) HyperTools: A python toolbox for gaining geometric insights into high-dimensional data. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2664,7 +2674,6 @@
           <t>Owen LLW, Manning JR (2017) A Gaussian process model of human ECoG data. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2687,7 +2696,6 @@
           <t>Ziman K, Heusser AC, Manning JR (2017) Effects of study context on recall organization. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2710,7 +2718,6 @@
           <t>Ziman K, Heusser AC, Manning JR (2017) Harnessing the power of mnemonic fingerprints: Maximizing learning potential by personalizing stimulus organization during adaptive list learning. &lt;em&gt;Context and Episodic Memory Symposium.&lt;/em&gt; Philadelphia, PA.</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2733,7 +2740,6 @@
           <t>Owen LLW, Manning JR (2017) Towards human super EEG. &lt;em&gt;Context and Episodic Memory Symposium.&lt;/em&gt; Philadelphia, PA.</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2756,7 +2762,6 @@
           <t>Heusser AC, Ziman K, Owen LLW, Manning JR (2017) HyperTools: A python toolbox for visualizing and manipulating high-dimensional data. &lt;em&gt;Context and Episodic Memory Symposium.&lt;/em&gt; Philadelphia, PA.</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2779,7 +2784,6 @@
           <t>Manning JR, Zhu Xia, Cohen J, Ranganath R, Stachenfeld K, Simony E, Regev M, Chen J, Hasson U, Willke T, Blei DM, Norman KA (2015) Exploring connectivity patterns in storytelling data using Hierarchical Topographic Factor Analysis (HTFA). &lt;em&gt;Collaborative Research in Computational Neuroscience&lt;/em&gt;. Seattle, WA.</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2802,7 +2806,6 @@
           <t>Manning JR, Stachenfeld K, Ranganath R, Norman KA, Blei DM (2014) Efficient discovery of functional brain networks in large multi-subject fMRI datasets. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2825,7 +2828,6 @@
           <t>Manning JR, Hulbert JC, Williams JA, Piloto LR, Sahakyan L, Norman KA (2014) Neural evidence for a context-change account of list-method directed forgetting. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2848,7 +2850,6 @@
           <t>Manning JR, Ranganath R, Blei DM, Norman KA (2014) Hierarchical Topographic Factor Analysis: a MATLAB toolbox for efficiently discovering brain networks in fMRI data. &lt;em&gt;Context and Episodic Memory Symposium.&lt;/em&gt; Philadelphia, PA.</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2871,7 +2872,6 @@
           <t>Manning JR, Blei DM, Norman KA (2013) Integrating neural and behavioral data into episodic memory models. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; San Diego, CA.</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2894,7 +2894,6 @@
           <t>Manning JR, Blei DM, Norman KA (2013) A probabilistic temporal context model for tracking mental context using neural and behavioral data. &lt;em&gt;Context and Episodic Memory Symposium.&lt;/em&gt; Philadelphia, PA. (Also presented at &lt;em&gt;Collaborative Research in Computational Neuroscience.&lt;/em&gt; Boston, MA)</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2917,7 +2916,6 @@
           <t>Manning JR, Gershman SJ, Blei DM, Norman KA (2012) Factor topographic latent source analysis: factor analysis for brain images. &lt;em&gt;Neural Information Processing Systems Machine Learning in NeuroImaging Workshop.&lt;/em&gt; Lake Tahoe, NV.</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2940,7 +2938,6 @@
           <t>Li N, Manning JR, Kahana MJ (2012) Decoding task and location information from multi-unit and local field potential activity. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; New Orleans, LA.</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2963,7 +2960,6 @@
           <t>Ramayya AG, Manning JR, Jacobs J, Fried I, Kahana MJ (2012) Distinct neuronal contributions to high frequency power changes in human local field potential recordings. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; New Orleans, LA.</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2986,7 +2982,6 @@
           <t>Manning JR, Blei DM, Norman KA (2012) Decoding topic vectors during memory encoding and retrieval. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; New Orleans, LA.</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3009,7 +3004,6 @@
           <t>Manning JR, Blei DM, Norman KA (2012) Text, neuroimaging, and memory: unified models of corpora and cognition. &lt;em&gt;Context and Episodic Memory Symposium.&lt;/em&gt; Philadelphia, PA.</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3032,7 +3026,6 @@
           <t>Manning JR, Polyn SM, Kahana MJ (2011) Tracking item representations during free recall. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3055,7 +3048,6 @@
           <t>Manning JR, Polyn SM, Kahana MJ (2010) How does the brain represent and retrieve word meanings? &lt;em&gt;Society for Neuroscience.&lt;/em&gt; San Diego, CA.</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3078,7 +3070,6 @@
           <t>Manning JR, Ranganath R, Keung W, Turk-Browne N, Norman KA, Blei DM (2010) New tools for decoding mental representations from neuroimaging data. &lt;em&gt;Cognitive Computational Neuroscience Conference.&lt;/em&gt; Philadelphia, PA.</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3101,7 +3092,6 @@
           <t>Manning JR, Polyn SM, Kahana MJ (2010) How does the brain represent and retrieve word meanings? &lt;em&gt;Architectures of Memory: Linking Systems and Cellular Neuroscience Workshop.&lt;/em&gt; Philadelphia, PA.</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3124,7 +3114,6 @@
           <t>Manning JR, Polyn SM, Kahana MJ (2009) Temporal and frontal networks reveal how conceptual memories are organized. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Chicago, IL.</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3147,7 +3136,6 @@
           <t>Benson NC, Manning JR, Brainard DH (2009) Learning receptor types from receptor responses. &lt;em&gt;Vision Sciences Society.&lt;/em&gt; Naples, FL.</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3170,7 +3158,6 @@
           <t>Manning JR, Jacobs J, Fried I, Kahana MJ (2009) The firing rate-LFP relation changes as a function of firing rate in humans. &lt;em&gt;Organization for Human Brain Mapping.&lt;/em&gt; San Francisco, CA.</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3193,7 +3180,6 @@
           <t>Manning JR, Polyn SM, Kahana MJ (2008) A neural signature of mental time travel. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3216,7 +3202,6 @@
           <t>Manning JR, Polyn SM, Kahana MJ (2007) Observing mental time travel in action: neurophysiological support for context-based models of episodic memory. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; San Diego, CA.</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3239,7 +3224,6 @@
           <t>Manning JR, Polyn SM, Kahana MJ (2007) Neural correlates of context-based models of free recall. &lt;em&gt;Cognitive Neuroscience Society.&lt;/em&gt; New York, NY.</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3262,7 +3246,6 @@
           <t>Manning JR, Polyn SM, Kahana MJ (2006) The neural representation of context and its role in free recall. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Atlanta, GA.</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3285,7 +3268,6 @@
           <t>Manning JR, Jacobs J, Fried I, Kahana MJ (2005) Broadband shifts in EEG power spectra are correlated with single-neuron activity in humans. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3308,7 +3290,6 @@
           <t>Manning JR, Lew TF, Brockman D, Li N, Kahana MJ (2005) An ideal navigator model of human wayfinding: learning one's way around a new town. &lt;em&gt;Cognitive Neuroscience Society.&lt;/em&gt; New York, NY.</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3331,7 +3312,44 @@
           <t>Manning JR, Brainard DH (2004) Why don't we see color at night? &lt;em&gt;Vision Sciences Society.&lt;/em&gt; Sarasota, FL.</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Translating neurophysiological recordings into dynamic estimates of conceptual knowledge and learning</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://digitalcommons.dartmouth.edu/wetterhahn_2024/15/</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Carstensen DL, Manning JR, Mucha P (2024) Translating neurophysiological recordings into dynamic estimates of conceptual knowledge and learning. &lt;em&gt;Wetterhahn Science Symposium&lt;/em&gt;, Hanover, NH.</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Exploring high-order network dynamics in brains and stock markets</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://digitalcommons.dartmouth.edu/wetterhahn_2023/4/</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Jha K, Carstensen DL, Patel A, Manning JR (2023) Exploring high-order network dynamics in brains and stock markets. &lt;em&gt;Wetterhahn Science Symposium&lt;/em&gt;, Hanover, NH.</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add dissertation PDFs and update spreadsheet with images/links
Dissertations added:
- Owen LLW (2021): Modeling the fast-timescale network dynamics that underlie complex thought
  - Image: timecorr.png
  - PDF: data/pdfs/owen_dissertation.pdf

- Ziman K (2022): Attending and remembering the external world
  - Image: ZimaEtAl19-34.png (attention timescale paper)
  - PDF: data/pdfs/ziman_dissertation.pdf

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/publications.xlsx
+++ b/data/publications.xlsx
@@ -1701,34 +1701,48 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>timecorr.png</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>Modeling the fast-timescale network dynamics that underlie complex thought</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>data/pdfs/owen_dissertation.pdf</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>Owen LLW (2021) Modeling the fast-timescale network dynamics that underlie complex thought. &lt;em&gt;Doctoral dissertation: Dartmouth College&lt;/em&gt;, Hanover, NH.</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ZimaEtAl19-34.png</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>Attending and remembering the external world</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>data/pdfs/ziman_dissertation.pdf</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>Ziman K (2022) Attending and remembering the external world. &lt;em&gt;Doctoral dissertation: Dartmouth College&lt;/em&gt;, Hanover, NH.</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3314,7 +3328,6 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
           <t>Translating neurophysiological recordings into dynamic estimates of conceptual knowledge and learning</t>
@@ -3330,10 +3343,8 @@
           <t>Carstensen DL, Manning JR, Mucha P (2024) Translating neurophysiological recordings into dynamic estimates of conceptual knowledge and learning. &lt;em&gt;Wetterhahn Science Symposium&lt;/em&gt;, Hanover, NH.</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
           <t>Exploring high-order network dynamics in brains and stock markets</t>
@@ -3349,7 +3360,6 @@
           <t>Jha K, Carstensen DL, Patel A, Manning JR (2023) Exploring high-order network dynamics in brains and stock markets. &lt;em&gt;Wetterhahn Science Symposium&lt;/em&gt;, Hanover, NH.</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add 9 new poster PDFs and update publications spreadsheet
Added PDFs for posters from multiple conferences:
- Wetterhahn 2025: Peng et al. (EEG knowledge tracking)
- OHBM 2022: Saggar et al. (Higher-order brain interactions)
- CCN 2022: Jain et al. (Cognitive markers mental health)
- CEMS 2020: Owen et al. (ECoG Gaussian process), Owen & Manning (Brain complexity)
- CEMS 2021: Xu et al. (Past/future inference)
- CEMS 2023: Xu & Manning (Statistical mechanics time)
- CEMS 2025: Xu & Manning (Temporal asymmetries)
- SfN 2021: Ziman & Manning (False familiarity)

Also added PDF links to existing Wetterhahn 2023/2024 entries.

Total publications: 122 (58 posters)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/publications.xlsx
+++ b/data/publications.xlsx
@@ -2361,7 +2361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ziman K, Lee MR, Martinez AR, Manning JR (2019) Volitional Attention Modulates Memory Encoding and Retrieval. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Chicago, IL</t>
+          <t>Ziman K, Lee MR, Martinez AR, Manning JR (2019) Volitional Attention Modulates Memory Encoding and Retrieval. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Chicago, IL. 792.22/LLL18.</t>
         </is>
       </c>
     </row>
@@ -2443,7 +2443,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Fitzpatrick PC, Heusser AC, Manning JR (2019) Exploring the evolving geometric structure of experiences and memories. &lt;em&gt;Society for Neuroscience&lt;/em&gt;. Chicago, IL.</t>
+          <t>Fitzpatrick PC, Heusser AC, Manning JR (2019) Exploring the evolving geometric structure of experiences and memories. &lt;em&gt;Society for Neuroscience&lt;/em&gt;. Chicago, IL. 423.16/BB14.</t>
         </is>
       </c>
     </row>
@@ -2465,7 +2465,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Owen LLW, Manning JR (2019) Understanding complexity and interactivity of brain patterns in naturalistic processing. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Chicago, IL.</t>
+          <t>Owen LLW, Manning JR (2019) Understanding complexity and interactivity of brain patterns in naturalistic processing. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Chicago, IL. 248.17/Z41.</t>
         </is>
       </c>
     </row>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ziman K, Lee MR, Martinez AR, Manning JR (2018) Volitional Attention Modulates Memory Encoding and Retrieval. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; San Diego, CA.</t>
+          <t>Ziman K, Lee MR, Martinez AR, Manning JR (2018) Volitional Attention Modulates Memory Encoding and Retrieval. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; San Diego, CA. 792.22/LLL18.</t>
         </is>
       </c>
     </row>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Fitzpatrick PC, Heusser AC, Manning JR (2018) Mapping between naturalistic experience and verbal recall. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; San Diego, CA.</t>
+          <t>Fitzpatrick PC, Heusser AC, Manning JR (2018) Mapping between naturalistic experience and verbal recall. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; San Diego, CA. 086.10/HHH33.</t>
         </is>
       </c>
     </row>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Manning JR, Ziman K, Heusser AC (2017) Efficient Learning: Manipulating context to enhance (or diminish) memory. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
+          <t>Manning JR, Ziman K, Heusser AC (2017) Efficient Learning: Manipulating context to enhance (or diminish) memory. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC. 339.08/UU42.</t>
         </is>
       </c>
     </row>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Heusser AC, Ziman K, Owen LLW, Manning JR (2017) HyperTools: A python toolbox for gaining geometric insights into high-dimensional data. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
+          <t>Heusser AC, Ziman K, Owen LLW, Manning JR (2017) HyperTools: A python toolbox for gaining geometric insights into high-dimensional data. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC. 721.22/WW28.</t>
         </is>
       </c>
     </row>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Owen LLW, Manning JR (2017) A Gaussian process model of human ECoG data. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
+          <t>Owen LLW, Manning JR (2017) A Gaussian process model of human ECoG data. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC. 093.04/UU78.</t>
         </is>
       </c>
     </row>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Ziman K, Heusser AC, Manning JR (2017) Effects of study context on recall organization. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC.</t>
+          <t>Ziman K, Heusser AC, Manning JR (2017) Effects of study context on recall organization. &lt;em&gt;Society for Neuroscience.&lt;/em&gt; Washington, DC. 803.07/UU14.</t>
         </is>
       </c>
     </row>
@@ -3343,6 +3343,11 @@
           <t>Carstensen DL, Manning JR, Mucha P (2024) Translating neurophysiological recordings into dynamic estimates of conceptual knowledge and learning. &lt;em&gt;Wetterhahn Science Symposium&lt;/em&gt;, Hanover, NH.</t>
         </is>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/CarsEtal24.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="B45" t="inlineStr">
@@ -3358,6 +3363,242 @@
       <c r="D45" t="inlineStr">
         <is>
           <t>Jha K, Carstensen DL, Patel A, Manning JR (2023) Exploring high-order network dynamics in brains and stock markets. &lt;em&gt;Wetterhahn Science Symposium&lt;/em&gt;, Hanover, NH.</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/JhaEtal23.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Episodic memory: Mental time travel or a quantum "memory wave" function?</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Manning JR (2019) Episodic memory: Mental time travel or a quantum "memory wave" function? &lt;em&gt;Context and Episodic Memory Symposium&lt;/em&gt;, Philadelphia, PA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>A geometric approach to modeling knowledge and learning from Khan Academy course videos</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Fitzpatrick PC, Heusser AC, Manning JR (2022) A geometric approach to modeling knowledge and learning from Khan Academy course videos. &lt;em&gt;Context and Episodic Memory Symposium&lt;/em&gt;, Philadelphia, PA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Temporal asymmetries in narrative events</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Xu X (2022) Temporal asymmetries in narrative events. &lt;em&gt;Context and Episodic Memory Symposium&lt;/em&gt;, Philadelphia, PA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Modeling the knowledge asymmetry of the past and the future</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Xu X (2024) Modeling the knowledge asymmetry of the past and the future. &lt;em&gt;Context and Episodic Memory Symposium&lt;/em&gt;, Philadelphia, PA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Shared representational geometry as an explanation for cross-subject prediction of place cell data from the rodent hippocampus</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Chen HT, Manning JR, van der Meer MAA (2019) Shared representational geometry as an explanation for cross-subject prediction of place cell data from the rodent hippocampus. &lt;em&gt;Society for Neuroscience&lt;/em&gt;, Chicago, IL. 084.04/Y28.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Translating neurophysiological recordings into dynamic estimates of conceptual knowledge and learning</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Peng K, Carstensen D, Parigela S, Shah O, Wingo A, Liu A, Maina J, Dampal K, Manning JR (2025) Translating neurophysiological recordings into dynamic estimates of conceptual knowledge and learning. &lt;em&gt;Karen E. Wetterhahn Science Symposium&lt;/em&gt;, Hanover, NH.</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/PengEtal25.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Higher-order interactions between brain regions are better at profiling tasks</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Saggar M, Betzel R, Manning JR, Liegeois R, Sporns O, Petri G (2022) Higher-order interactions between brain regions are better at profiling tasks. &lt;em&gt;Organization for Human Brain Mapping&lt;/em&gt;, Glasgow, Scotland.</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/SaggEtal22.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Cognitive markers of mental health</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Jain S, Schreder N, Fitzpatrick PC, Ziman K, Manning JR (2022) Cognitive markers of mental health. &lt;em&gt;Conference on Cognitive Computational Neuroscience&lt;/em&gt;, San Francisco, CA.</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/JainEtal22.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>A Gaussian process model of human ECoG data</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Owen LLW, Muntianu TA, Heusser AC, Manning JR (2020) A Gaussian process model of human ECoG data. &lt;em&gt;Context and Episodic Memory Symposium&lt;/em&gt;, Philadelphia, PA (virtual).</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/OwenEtal20.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Understanding brain pattern complexity and interactivity in naturalistic processing</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Owen LLW, Manning JR (2020) Understanding brain pattern complexity and interactivity in naturalistic processing. &lt;em&gt;Context and Episodic Memory Symposium&lt;/em&gt;, Philadelphia, PA (virtual).</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/OwenMann20.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Extrapolating the unobserved past and future in other people's autobiographical timelines</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Xu X, Zhu Z, Manning JR (2021) Extrapolating the unobserved past and future in other people's autobiographical timelines. &lt;em&gt;Context and Episodic Memory Symposium&lt;/em&gt;, Philadelphia, PA.</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/XuEtal21.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Why we know more about the past: insights from statistical mechanics</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Xu X, Manning JR (2023) Why we know more about the past: insights from statistical mechanics. &lt;em&gt;Context and Episodic Memory Symposium&lt;/em&gt;, Orlando, FL.</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/XuMann23.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Temporal asymmetries in cued recall of naturalistic events</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Xu X, Manning JR (2025) Temporal asymmetries in cued recall of naturalistic events. &lt;em&gt;Context and Episodic Memory Symposium&lt;/em&gt;, Philadelphia, PA.</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/XuMann25.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Unexpected false feelings of familiarity about faces are associated with increased pupil dilations</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Ziman K, Manning JR (2021) Unexpected false feelings of familiarity about faces are associated with increased pupil dilations. &lt;em&gt;Society for Neuroscience&lt;/em&gt;, Virtual.</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>[&lt;a href="data/pdfs/ZimaMann21.pdf" target="_blank"&gt;pdf&lt;/a&gt;]</t>
         </is>
       </c>
     </row>

</xml_diff>